<commit_message>
completed the final output portion, still having issues with forced task
</commit_message>
<xml_diff>
--- a/python/output_pretest/pretest_Alex.xlsx
+++ b/python/output_pretest/pretest_Alex.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="37">
   <si>
     <t>ORTHO TARGET</t>
   </si>
@@ -31,109 +31,100 @@
     <t>Kinesin</t>
   </si>
   <si>
+    <t>Reducer</t>
+  </si>
+  <si>
+    <t>Isotope</t>
+  </si>
+  <si>
+    <t>Oxidizer</t>
+  </si>
+  <si>
+    <t>Eukaryote</t>
+  </si>
+  <si>
+    <t>Phosphorylation</t>
+  </si>
+  <si>
+    <t>Cytoplasm</t>
+  </si>
+  <si>
+    <t>Ribosomes</t>
+  </si>
+  <si>
     <t>Glycolysis</t>
   </si>
   <si>
+    <t>Chlorophyll</t>
+  </si>
+  <si>
+    <t>Dynein</t>
+  </si>
+  <si>
+    <t>Isotonic</t>
+  </si>
+  <si>
+    <t>Nucleoid</t>
+  </si>
+  <si>
+    <t>Tertiary</t>
+  </si>
+  <si>
+    <t>Exergonic</t>
+  </si>
+  <si>
+    <t>Ribonucleoside</t>
+  </si>
+  <si>
+    <t>Purine</t>
+  </si>
+  <si>
+    <t>Quaternary</t>
+  </si>
+  <si>
+    <t>Catalyst</t>
+  </si>
+  <si>
+    <t>Desmosomes</t>
+  </si>
+  <si>
+    <t>Amphipathic</t>
+  </si>
+  <si>
+    <t>Monosaccharides</t>
+  </si>
+  <si>
+    <t>Peroxisome</t>
+  </si>
+  <si>
+    <t>Chemiosmotic</t>
+  </si>
+  <si>
+    <t>Hypertonic</t>
+  </si>
+  <si>
     <t>Microtubule</t>
   </si>
   <si>
-    <t>Chlorophyll</t>
-  </si>
-  <si>
-    <t>Tertiary</t>
-  </si>
-  <si>
-    <t>Peroxisome</t>
-  </si>
-  <si>
-    <t>Isotope</t>
-  </si>
-  <si>
-    <t>Oxidizer</t>
-  </si>
-  <si>
-    <t>Hypertonic</t>
-  </si>
-  <si>
-    <t>Catalyst</t>
-  </si>
-  <si>
-    <t>Amphipathic</t>
-  </si>
-  <si>
-    <t>Cytoplasm</t>
-  </si>
-  <si>
-    <t>Isotonic</t>
+    <t>Centrioles</t>
+  </si>
+  <si>
+    <t>Vacuole</t>
   </si>
   <si>
     <t>Lysosome</t>
   </si>
   <si>
-    <t>Monosaccharides</t>
-  </si>
-  <si>
-    <t>Ribosomes</t>
-  </si>
-  <si>
-    <t>Chemiosmotic</t>
-  </si>
-  <si>
-    <t>Vacuole</t>
-  </si>
-  <si>
-    <t>Dynein</t>
-  </si>
-  <si>
-    <t>Desmosomes</t>
-  </si>
-  <si>
     <t>Nucleotides</t>
   </si>
   <si>
-    <t>Quaternary</t>
-  </si>
-  <si>
-    <t>Ribonucleoside</t>
-  </si>
-  <si>
-    <t>Centrioles</t>
-  </si>
-  <si>
-    <t>Phosphorylation</t>
-  </si>
-  <si>
-    <t>Reducer</t>
-  </si>
-  <si>
-    <t>Nucleoid</t>
-  </si>
-  <si>
-    <t>Exergonic</t>
-  </si>
-  <si>
-    <t>Purine</t>
-  </si>
-  <si>
-    <t>Eukaryote</t>
-  </si>
-  <si>
-    <t>Ala</t>
-  </si>
-  <si>
-    <t>ala</t>
-  </si>
-  <si>
-    <t>lala</t>
-  </si>
-  <si>
-    <t>a</t>
+    <t>s</t>
+  </si>
+  <si>
+    <t>low</t>
   </si>
   <si>
     <t>high</t>
-  </si>
-  <si>
-    <t>low</t>
   </si>
 </sst>
 </file>
@@ -525,7 +516,7 @@
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -536,13 +527,13 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -553,13 +544,13 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -570,13 +561,13 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -587,13 +578,13 @@
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -604,13 +595,13 @@
         <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -621,13 +612,13 @@
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D8">
         <v>0</v>
       </c>
       <c r="E8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -638,13 +629,13 @@
         <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D9">
         <v>0</v>
       </c>
       <c r="E9" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -655,13 +646,13 @@
         <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D10">
         <v>0</v>
       </c>
       <c r="E10" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -672,13 +663,13 @@
         <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D11">
         <v>0</v>
       </c>
       <c r="E11" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -689,13 +680,13 @@
         <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D12">
         <v>0</v>
       </c>
       <c r="E12" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -706,13 +697,13 @@
         <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D13">
         <v>0</v>
       </c>
       <c r="E13" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -723,13 +714,13 @@
         <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D14">
         <v>0</v>
       </c>
       <c r="E14" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -740,13 +731,13 @@
         <v>17</v>
       </c>
       <c r="C15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D15">
         <v>0</v>
       </c>
       <c r="E15" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -757,13 +748,13 @@
         <v>18</v>
       </c>
       <c r="C16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D16">
         <v>0</v>
       </c>
       <c r="E16" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -774,13 +765,13 @@
         <v>19</v>
       </c>
       <c r="C17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D17">
         <v>0</v>
       </c>
       <c r="E17" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -791,13 +782,13 @@
         <v>20</v>
       </c>
       <c r="C18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D18">
         <v>0</v>
       </c>
       <c r="E18" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -808,13 +799,13 @@
         <v>21</v>
       </c>
       <c r="C19" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D19">
         <v>0</v>
       </c>
       <c r="E19" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -825,13 +816,13 @@
         <v>22</v>
       </c>
       <c r="C20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D20">
         <v>0</v>
       </c>
       <c r="E20" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -842,13 +833,13 @@
         <v>23</v>
       </c>
       <c r="C21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D21">
         <v>0</v>
       </c>
       <c r="E21" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -859,13 +850,13 @@
         <v>24</v>
       </c>
       <c r="C22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D22">
         <v>0</v>
       </c>
       <c r="E22" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -876,13 +867,13 @@
         <v>25</v>
       </c>
       <c r="C23" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D23">
         <v>0</v>
       </c>
       <c r="E23" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -893,13 +884,13 @@
         <v>26</v>
       </c>
       <c r="C24" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D24">
         <v>0</v>
       </c>
       <c r="E24" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -910,13 +901,13 @@
         <v>27</v>
       </c>
       <c r="C25" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D25">
         <v>0</v>
       </c>
       <c r="E25" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -927,13 +918,13 @@
         <v>28</v>
       </c>
       <c r="C26" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D26">
         <v>0</v>
       </c>
       <c r="E26" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -944,13 +935,13 @@
         <v>29</v>
       </c>
       <c r="C27" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D27">
         <v>0</v>
       </c>
       <c r="E27" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -961,13 +952,13 @@
         <v>30</v>
       </c>
       <c r="C28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D28">
         <v>0</v>
       </c>
       <c r="E28" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -978,13 +969,13 @@
         <v>31</v>
       </c>
       <c r="C29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D29">
         <v>0</v>
       </c>
       <c r="E29" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -995,13 +986,13 @@
         <v>32</v>
       </c>
       <c r="C30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D30">
         <v>0</v>
       </c>
       <c r="E30" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -1012,13 +1003,13 @@
         <v>33</v>
       </c>
       <c r="C31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D31">
         <v>0</v>
       </c>
       <c r="E31" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>